<commit_message>
feat(global): 📝 document more issues
</commit_message>
<xml_diff>
--- a/list_of_issues.xlsx
+++ b/list_of_issues.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/Coding/TransitionZero/pypsa-earth-trace/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F514F4C9-13E6-4943-842C-5577948A6404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="6260" yWindow="760" windowWidth="16380" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Country</t>
   </si>
@@ -56,13 +62,27 @@
   </si>
   <si>
     <t xml:space="preserve">Seemingly because Sudan doesn't have line data although openinframap shows that it does. </t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is data here. Again OSM processing issue that needs to be addressed. </t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Issues with getting the data from OSM. Cables again</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,38 +125,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -147,10 +158,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -188,71 +199,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -280,7 +291,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -303,11 +314,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -316,13 +327,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -332,7 +343,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -341,7 +352,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -350,7 +361,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -358,10 +369,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -426,74 +437,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="53.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="64.5" customFormat="1" s="3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="29.25" customFormat="1" s="3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="29.25" customFormat="1" s="3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="40.5" customFormat="1" s="3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(global): 📝 update list of issues
</commit_message>
<xml_diff>
--- a/list_of_issues.xlsx
+++ b/list_of_issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/Coding/TransitionZero/pypsa-earth-trace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F514F4C9-13E6-4943-842C-5577948A6404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4275D5C-94BF-6145-8D47-6163FAB65166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="760" windowWidth="16380" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Country</t>
   </si>
@@ -77,6 +77,21 @@
   </si>
   <si>
     <t>Issues with getting the data from OSM. Cables again</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Gabon</t>
   </si>
 </sst>
 </file>
@@ -441,10 +456,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -536,6 +551,46 @@
         <v>18</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(global): 📝 add more issues
</commit_message>
<xml_diff>
--- a/list_of_issues.xlsx
+++ b/list_of_issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/Coding/TransitionZero/pypsa-earth-trace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4275D5C-94BF-6145-8D47-6163FAB65166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C457E2AA-2926-3447-A3F9-DA5FA395C47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6260" yWindow="760" windowWidth="16380" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Country</t>
   </si>
@@ -92,6 +92,45 @@
   </si>
   <si>
     <t>Gabon</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Issue with Nan numbers when building shapes. Also the OSM data seems to span multiple countries.</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>OSM issue with cables</t>
+  </si>
+  <si>
+    <t>Burkina Fasso</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guinea Bissau</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>No powerplants so ppmatching breaks</t>
+  </si>
+  <si>
+    <t>Madgascar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malawi </t>
   </si>
 </sst>
 </file>
@@ -456,10 +495,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -591,6 +630,86 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(global): 📝 update model progress and issues
</commit_message>
<xml_diff>
--- a/list_of_issues.xlsx
+++ b/list_of_issues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/Coding/TransitionZero/pypsa-earth-trace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA8C280-D0A5-8249-8910-EDB36BC3E187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C34E4A-7AE5-5040-B3AB-320B0686B49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="760" windowWidth="22560" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4580" yWindow="800" windowWidth="25420" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Country</t>
   </si>
@@ -131,6 +131,24 @@
   </si>
   <si>
     <t xml:space="preserve">Malawi </t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Equitorial Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burundi </t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>New Caledonia</t>
+  </si>
+  <si>
+    <t>Guyana</t>
   </si>
 </sst>
 </file>
@@ -495,10 +513,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="171" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -710,6 +728,54 @@
         <v>28</v>
       </c>
     </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore(global): 📝 update list of issues
</commit_message>
<xml_diff>
--- a/list_of_issues.xlsx
+++ b/list_of_issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/Coding/TransitionZero/pypsa-earth-trace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C34E4A-7AE5-5040-B3AB-320B0686B49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6765AA-2CE2-A947-8F4A-26ADDA617878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4580" yWindow="800" windowWidth="25420" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>Country</t>
   </si>
@@ -149,6 +149,39 @@
   </si>
   <si>
     <t>Guyana</t>
+  </si>
+  <si>
+    <t>HongKong</t>
+  </si>
+  <si>
+    <t>Issue with OSM rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azerbeijan </t>
+  </si>
+  <si>
+    <t>Issues with OSM cables</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Cutout seems to be too large. Need to look into this</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Armenia</t>
   </si>
 </sst>
 </file>
@@ -513,10 +546,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="171" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="171" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -776,6 +809,70 @@
         <v>28</v>
       </c>
     </row>
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>